<commit_message>
catégorie ok manque stocke available
</commit_message>
<xml_diff>
--- a/Test Import Presta M20S.xlsx
+++ b/Test Import Presta M20S.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t xml:space="preserve">Titre</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">truc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new</t>
   </si>
 </sst>
 </file>
@@ -288,8 +291,8 @@
   </sheetPr>
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -452,7 +455,7 @@
         <v>1</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="n">
@@ -495,8 +498,8 @@
       <c r="AC2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AD2" s="1" t="n">
-        <v>1</v>
+      <c r="AD2" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="AE2" s="1" t="n">
         <v>1</v>

</xml_diff>